<commit_message>
commit after xl change
</commit_message>
<xml_diff>
--- a/ds_algo/src/test/resources/ExcelData/sample.xlsx
+++ b/ds_algo/src/test/resources/ExcelData/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umara\eclipse-workspace\ds_algo\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umara\git\ds-algo\ds_algo\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0608C1BA-2B68-47FC-A4E4-C7A50C4E2A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F3A5A8-EDE7-4C03-B97D-A4FACD9610CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A1275A8F-F8E5-194E-9D5F-EB87A35A82C7}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>[4, 9, 9, 49, 121]</t>
   </si>
   <si>
-    <t>Welcome to the demo</t>
-  </si>
-  <si>
     <t>pythoncode</t>
   </si>
   <si>
@@ -151,10 +148,13 @@
     <t>temp12!@</t>
   </si>
   <si>
-    <t>print("Welcome to the DS-Algo demo");</t>
-  </si>
-  <si>
     <t>print(Invalid code);</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>print("Welcome");</t>
   </si>
 </sst>
 </file>
@@ -566,21 +566,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -588,10 +588,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -599,10 +599,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -619,7 +619,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -631,23 +631,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>